<commit_message>
Changes in POM Page
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANSHUMAN SINGH\Downloads\AppFincart-20210907T080953Z-001\AppFincart\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANSHUMAN SINGH\git\Azure-Selenium-Demo\AppFincart\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EE3CA8-72A5-4F07-8C4B-91465CCAF95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035EA95F-86C3-444C-8B56-CBB77A510789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{B486DD6E-9D6E-4328-9ABF-86CE64B531DF}"/>
   </bookViews>
@@ -92,10 +92,10 @@
     <t>pan</t>
   </si>
   <si>
-    <t>testweb16july22@gmail.com</t>
-  </si>
-  <si>
-    <t>TEEPT2091I</t>
+    <t>testweb30july22@gmail.com</t>
+  </si>
+  <si>
+    <t>TEEPT2091J</t>
   </si>
 </sst>
 </file>

</xml_diff>